<commit_message>
updates layout for use of control sample_id
</commit_message>
<xml_diff>
--- a/data-raw/exampleoutput_synergyH1trial_data_092021.xlsx
+++ b/data-raw/exampleoutput_synergyH1trial_data_092021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ef347\Box Sync\SHERLOCK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanuel\projects\jpe\grunID\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA10137-EFCD-4400-8613-0C92FA75793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992DB9F-C060-4AFE-A486-3B1288A508F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="9465" windowHeight="10380"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -808,11 +808,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:W145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="V114" sqref="V114:V119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>